<commit_message>
Updated Ingredient Simplifications through line 1237 (leaving only ingredients with frequencies less than 100)
</commit_message>
<xml_diff>
--- a/Nathan_notebooks/ingredient_data/manually_generated_ingredient_simplification_spreadsheet_sorted_by_popularity_in_progress.xlsx
+++ b/Nathan_notebooks/ingredient_data/manually_generated_ingredient_simplification_spreadsheet_sorted_by_popularity_in_progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/20677176c3140885/O-D Documents/Coding Projects/Learning/Erdos Institute/Group Project May 2024/foodrecs/Nathan_notebooks/ingredient_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="477" documentId="8_{BE6724C2-2954-4F7A-9241-F6ECE9C0BD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D85EBC23-9AA1-4C1B-8F6A-58DCE35D0275}"/>
+  <xr:revisionPtr revIDLastSave="823" documentId="8_{BE6724C2-2954-4F7A-9241-F6ECE9C0BD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBFCD937-2663-49EB-B290-EC44646C4A1E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10371" uniqueCount="5367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10371" uniqueCount="5412">
   <si>
     <t>original</t>
   </si>
@@ -16134,6 +16134,141 @@
   </si>
   <si>
     <t>basil, pesto</t>
+  </si>
+  <si>
+    <t>red curry</t>
+  </si>
+  <si>
+    <t>pasilla chile</t>
+  </si>
+  <si>
+    <t>raspberry, vinegar</t>
+  </si>
+  <si>
+    <t>vanilla, vodka</t>
+  </si>
+  <si>
+    <t>liqueur</t>
+  </si>
+  <si>
+    <t>avocadoes</t>
+  </si>
+  <si>
+    <t>vegetable bouillon</t>
+  </si>
+  <si>
+    <t>vanilla, pudding</t>
+  </si>
+  <si>
+    <t>stuffing</t>
+  </si>
+  <si>
+    <t>garbonzos</t>
+  </si>
+  <si>
+    <t>lentil</t>
+  </si>
+  <si>
+    <t>catfish</t>
+  </si>
+  <si>
+    <t>chocolate, ice cream</t>
+  </si>
+  <si>
+    <t>garlic, oregano, turmeric</t>
+  </si>
+  <si>
+    <t>matzah</t>
+  </si>
+  <si>
+    <t>cucumber</t>
+  </si>
+  <si>
+    <t>chicken, stuffing</t>
+  </si>
+  <si>
+    <t>tarragon, vinegar</t>
+  </si>
+  <si>
+    <t>tamarind</t>
+  </si>
+  <si>
+    <t>red pepper</t>
+  </si>
+  <si>
+    <t>scallop</t>
+  </si>
+  <si>
+    <t>vital wheat gluten, flour</t>
+  </si>
+  <si>
+    <t>sriracha</t>
+  </si>
+  <si>
+    <t>liquor</t>
+  </si>
+  <si>
+    <t>halibut</t>
+  </si>
+  <si>
+    <t>almonds</t>
+  </si>
+  <si>
+    <t>monterey jack cheese, cheddar cheese</t>
+  </si>
+  <si>
+    <t>bone</t>
+  </si>
+  <si>
+    <t>cinnamon, nutmeg</t>
+  </si>
+  <si>
+    <t>kidney beans</t>
+  </si>
+  <si>
+    <t>sole</t>
+  </si>
+  <si>
+    <t>butterscotch, pudding</t>
+  </si>
+  <si>
+    <t>chili peppers</t>
+  </si>
+  <si>
+    <t>green olive</t>
+  </si>
+  <si>
+    <t>red currant, jelly</t>
+  </si>
+  <si>
+    <t>vanilla, soymilk</t>
+  </si>
+  <si>
+    <t>lime, gelatin</t>
+  </si>
+  <si>
+    <t>whipped cream</t>
+  </si>
+  <si>
+    <t>orange juice, orange zest</t>
+  </si>
+  <si>
+    <t>wheat</t>
+  </si>
+  <si>
+    <t>beets</t>
+  </si>
+  <si>
+    <t>fig</t>
+  </si>
+  <si>
+    <t>artichokes</t>
+  </si>
+  <si>
+    <t>raspberry, gelatin</t>
+  </si>
+  <si>
+    <t>lemon, pudding</t>
   </si>
 </sst>
 </file>
@@ -16239,6 +16374,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16526,10 +16665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5185"/>
+  <dimension ref="A1:C5185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A783" workbookViewId="0">
-      <selection activeCell="E802" sqref="E802"/>
+    <sheetView tabSelected="1" topLeftCell="A1206" workbookViewId="0">
+      <selection activeCell="B1238" sqref="B1238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20417,7 +20556,7 @@
         <v>358</v>
       </c>
       <c r="B353" t="s">
-        <v>5033</v>
+        <v>5186</v>
       </c>
       <c r="C353">
         <v>857</v>
@@ -25340,7 +25479,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="801" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="801" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A801" t="s">
         <v>813</v>
       </c>
@@ -25351,63 +25490,51 @@
         <v>236</v>
       </c>
     </row>
-    <row r="802" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="802" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A802" t="s">
         <v>814</v>
       </c>
-      <c r="B802" s="2" t="s">
+      <c r="B802" t="s">
         <v>137</v>
       </c>
       <c r="C802">
         <v>235</v>
       </c>
-      <c r="E802">
-        <f>SUM(C2:C802)</f>
-        <v>2004853</v>
-      </c>
-      <c r="G802">
-        <f>E803/(E802+E803)</f>
-        <v>6.0579934109259048E-2</v>
-      </c>
-    </row>
-    <row r="803" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="803" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A803" t="s">
         <v>815</v>
       </c>
       <c r="B803" t="s">
-        <v>815</v>
+        <v>749</v>
       </c>
       <c r="C803">
         <v>234</v>
       </c>
-      <c r="E803">
-        <f>SUM(C803:C5185)</f>
-        <v>129286</v>
-      </c>
-    </row>
-    <row r="804" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="804" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A804" t="s">
         <v>816</v>
       </c>
       <c r="B804" t="s">
-        <v>816</v>
+        <v>396</v>
       </c>
       <c r="C804">
         <v>234</v>
       </c>
     </row>
-    <row r="805" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="805" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A805" t="s">
         <v>817</v>
       </c>
       <c r="B805" t="s">
-        <v>817</v>
+        <v>894</v>
       </c>
       <c r="C805">
         <v>234</v>
       </c>
     </row>
-    <row r="806" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="806" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A806" t="s">
         <v>818</v>
       </c>
@@ -25418,29 +25545,29 @@
         <v>233</v>
       </c>
     </row>
-    <row r="807" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="807" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A807" t="s">
         <v>819</v>
       </c>
       <c r="B807" t="s">
-        <v>819</v>
+        <v>161</v>
       </c>
       <c r="C807">
         <v>233</v>
       </c>
     </row>
-    <row r="808" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="808" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A808" t="s">
         <v>820</v>
       </c>
       <c r="B808" t="s">
-        <v>820</v>
+        <v>191</v>
       </c>
       <c r="C808">
         <v>233</v>
       </c>
     </row>
-    <row r="809" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="809" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A809" t="s">
         <v>821</v>
       </c>
@@ -25451,7 +25578,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="810" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="810" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A810" t="s">
         <v>822</v>
       </c>
@@ -25462,7 +25589,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="811" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="811" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A811" t="s">
         <v>823</v>
       </c>
@@ -25473,51 +25600,51 @@
         <v>231</v>
       </c>
     </row>
-    <row r="812" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="812" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A812" t="s">
         <v>825</v>
       </c>
       <c r="B812" t="s">
-        <v>825</v>
+        <v>736</v>
       </c>
       <c r="C812">
         <v>231</v>
       </c>
     </row>
-    <row r="813" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="813" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A813" t="s">
         <v>826</v>
       </c>
       <c r="B813" t="s">
-        <v>826</v>
+        <v>307</v>
       </c>
       <c r="C813">
         <v>230</v>
       </c>
     </row>
-    <row r="814" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="814" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A814" t="s">
         <v>827</v>
       </c>
       <c r="B814" t="s">
-        <v>827</v>
+        <v>17</v>
       </c>
       <c r="C814">
         <v>230</v>
       </c>
     </row>
-    <row r="815" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="815" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A815" t="s">
         <v>828</v>
       </c>
       <c r="B815" t="s">
-        <v>828</v>
+        <v>5367</v>
       </c>
       <c r="C815">
         <v>229</v>
       </c>
     </row>
-    <row r="816" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="816" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A816" t="s">
         <v>829</v>
       </c>
@@ -25544,7 +25671,7 @@
         <v>831</v>
       </c>
       <c r="B818" t="s">
-        <v>831</v>
+        <v>12</v>
       </c>
       <c r="C818">
         <v>226</v>
@@ -25555,7 +25682,7 @@
         <v>832</v>
       </c>
       <c r="B819" t="s">
-        <v>832</v>
+        <v>5368</v>
       </c>
       <c r="C819">
         <v>225</v>
@@ -25566,7 +25693,7 @@
         <v>833</v>
       </c>
       <c r="B820" t="s">
-        <v>833</v>
+        <v>131</v>
       </c>
       <c r="C820">
         <v>225</v>
@@ -25610,7 +25737,7 @@
         <v>838</v>
       </c>
       <c r="B824" t="s">
-        <v>838</v>
+        <v>175</v>
       </c>
       <c r="C824">
         <v>224</v>
@@ -25632,7 +25759,7 @@
         <v>840</v>
       </c>
       <c r="B826" t="s">
-        <v>840</v>
+        <v>34</v>
       </c>
       <c r="C826">
         <v>222</v>
@@ -25643,7 +25770,7 @@
         <v>841</v>
       </c>
       <c r="B827" t="s">
-        <v>841</v>
+        <v>374</v>
       </c>
       <c r="C827">
         <v>222</v>
@@ -25654,7 +25781,7 @@
         <v>842</v>
       </c>
       <c r="B828" t="s">
-        <v>842</v>
+        <v>487</v>
       </c>
       <c r="C828">
         <v>222</v>
@@ -25665,7 +25792,7 @@
         <v>843</v>
       </c>
       <c r="B829" t="s">
-        <v>844</v>
+        <v>245</v>
       </c>
       <c r="C829">
         <v>222</v>
@@ -25676,7 +25803,7 @@
         <v>845</v>
       </c>
       <c r="B830" t="s">
-        <v>845</v>
+        <v>127</v>
       </c>
       <c r="C830">
         <v>222</v>
@@ -25698,7 +25825,7 @@
         <v>847</v>
       </c>
       <c r="B832" t="s">
-        <v>847</v>
+        <v>15</v>
       </c>
       <c r="C832">
         <v>221</v>
@@ -25709,7 +25836,7 @@
         <v>848</v>
       </c>
       <c r="B833" t="s">
-        <v>848</v>
+        <v>168</v>
       </c>
       <c r="C833">
         <v>220</v>
@@ -25720,7 +25847,7 @@
         <v>849</v>
       </c>
       <c r="B834" t="s">
-        <v>849</v>
+        <v>483</v>
       </c>
       <c r="C834">
         <v>219</v>
@@ -25753,7 +25880,7 @@
         <v>852</v>
       </c>
       <c r="B837" t="s">
-        <v>852</v>
+        <v>143</v>
       </c>
       <c r="C837">
         <v>218</v>
@@ -25775,7 +25902,7 @@
         <v>854</v>
       </c>
       <c r="B839" t="s">
-        <v>854</v>
+        <v>11</v>
       </c>
       <c r="C839">
         <v>217</v>
@@ -25786,7 +25913,7 @@
         <v>855</v>
       </c>
       <c r="B840" t="s">
-        <v>855</v>
+        <v>212</v>
       </c>
       <c r="C840">
         <v>217</v>
@@ -25797,7 +25924,7 @@
         <v>856</v>
       </c>
       <c r="B841" t="s">
-        <v>856</v>
+        <v>440</v>
       </c>
       <c r="C841">
         <v>217</v>
@@ -25819,7 +25946,7 @@
         <v>858</v>
       </c>
       <c r="B843" t="s">
-        <v>858</v>
+        <v>3</v>
       </c>
       <c r="C843">
         <v>216</v>
@@ -25830,7 +25957,7 @@
         <v>859</v>
       </c>
       <c r="B844" t="s">
-        <v>859</v>
+        <v>185</v>
       </c>
       <c r="C844">
         <v>215</v>
@@ -25841,7 +25968,7 @@
         <v>860</v>
       </c>
       <c r="B845" t="s">
-        <v>860</v>
+        <v>222</v>
       </c>
       <c r="C845">
         <v>215</v>
@@ -25863,7 +25990,7 @@
         <v>862</v>
       </c>
       <c r="B847" t="s">
-        <v>862</v>
+        <v>17</v>
       </c>
       <c r="C847">
         <v>215</v>
@@ -25874,7 +26001,7 @@
         <v>863</v>
       </c>
       <c r="B848" t="s">
-        <v>863</v>
+        <v>5369</v>
       </c>
       <c r="C848">
         <v>214</v>
@@ -25885,7 +26012,7 @@
         <v>864</v>
       </c>
       <c r="B849" t="s">
-        <v>864</v>
+        <v>226</v>
       </c>
       <c r="C849">
         <v>213</v>
@@ -25896,7 +26023,7 @@
         <v>865</v>
       </c>
       <c r="B850" t="s">
-        <v>865</v>
+        <v>87</v>
       </c>
       <c r="C850">
         <v>212</v>
@@ -25907,7 +26034,7 @@
         <v>866</v>
       </c>
       <c r="B851" t="s">
-        <v>866</v>
+        <v>4</v>
       </c>
       <c r="C851">
         <v>210</v>
@@ -25918,7 +26045,7 @@
         <v>867</v>
       </c>
       <c r="B852" t="s">
-        <v>116</v>
+        <v>867</v>
       </c>
       <c r="C852">
         <v>210</v>
@@ -25940,7 +26067,7 @@
         <v>869</v>
       </c>
       <c r="B854" t="s">
-        <v>869</v>
+        <v>222</v>
       </c>
       <c r="C854">
         <v>207</v>
@@ -25951,7 +26078,7 @@
         <v>870</v>
       </c>
       <c r="B855" t="s">
-        <v>870</v>
+        <v>548</v>
       </c>
       <c r="C855">
         <v>207</v>
@@ -25973,7 +26100,7 @@
         <v>871</v>
       </c>
       <c r="B857" t="s">
-        <v>871</v>
+        <v>736</v>
       </c>
       <c r="C857">
         <v>207</v>
@@ -26006,7 +26133,7 @@
         <v>874</v>
       </c>
       <c r="B860" t="s">
-        <v>874</v>
+        <v>465</v>
       </c>
       <c r="C860">
         <v>205</v>
@@ -26017,7 +26144,7 @@
         <v>875</v>
       </c>
       <c r="B861" t="s">
-        <v>875</v>
+        <v>5370</v>
       </c>
       <c r="C861">
         <v>204</v>
@@ -26028,7 +26155,7 @@
         <v>876</v>
       </c>
       <c r="B862" t="s">
-        <v>876</v>
+        <v>91</v>
       </c>
       <c r="C862">
         <v>204</v>
@@ -26050,7 +26177,7 @@
         <v>878</v>
       </c>
       <c r="B864" t="s">
-        <v>878</v>
+        <v>127</v>
       </c>
       <c r="C864">
         <v>204</v>
@@ -26072,7 +26199,7 @@
         <v>880</v>
       </c>
       <c r="B866" t="s">
-        <v>880</v>
+        <v>143</v>
       </c>
       <c r="C866">
         <v>203</v>
@@ -26083,7 +26210,7 @@
         <v>881</v>
       </c>
       <c r="B867" t="s">
-        <v>881</v>
+        <v>5371</v>
       </c>
       <c r="C867">
         <v>203</v>
@@ -26094,7 +26221,7 @@
         <v>882</v>
       </c>
       <c r="B868" t="s">
-        <v>882</v>
+        <v>245</v>
       </c>
       <c r="C868">
         <v>202</v>
@@ -26105,7 +26232,7 @@
         <v>883</v>
       </c>
       <c r="B869" t="s">
-        <v>883</v>
+        <v>4804</v>
       </c>
       <c r="C869">
         <v>202</v>
@@ -26116,7 +26243,7 @@
         <v>884</v>
       </c>
       <c r="B870" t="s">
-        <v>884</v>
+        <v>736</v>
       </c>
       <c r="C870">
         <v>202</v>
@@ -26138,7 +26265,7 @@
         <v>886</v>
       </c>
       <c r="B872" t="s">
-        <v>886</v>
+        <v>279</v>
       </c>
       <c r="C872">
         <v>200</v>
@@ -26149,7 +26276,7 @@
         <v>887</v>
       </c>
       <c r="B873" t="s">
-        <v>887</v>
+        <v>39</v>
       </c>
       <c r="C873">
         <v>199</v>
@@ -26160,7 +26287,7 @@
         <v>888</v>
       </c>
       <c r="B874" t="s">
-        <v>888</v>
+        <v>91</v>
       </c>
       <c r="C874">
         <v>198</v>
@@ -26171,7 +26298,7 @@
         <v>889</v>
       </c>
       <c r="B875" t="s">
-        <v>889</v>
+        <v>532</v>
       </c>
       <c r="C875">
         <v>198</v>
@@ -26182,7 +26309,7 @@
         <v>890</v>
       </c>
       <c r="B876" t="s">
-        <v>890</v>
+        <v>915</v>
       </c>
       <c r="C876">
         <v>198</v>
@@ -26193,7 +26320,7 @@
         <v>891</v>
       </c>
       <c r="B877" t="s">
-        <v>891</v>
+        <v>5372</v>
       </c>
       <c r="C877">
         <v>197</v>
@@ -26204,7 +26331,7 @@
         <v>892</v>
       </c>
       <c r="B878" t="s">
-        <v>892</v>
+        <v>226</v>
       </c>
       <c r="C878">
         <v>196</v>
@@ -26237,7 +26364,7 @@
         <v>895</v>
       </c>
       <c r="B881" t="s">
-        <v>895</v>
+        <v>107</v>
       </c>
       <c r="C881">
         <v>195</v>
@@ -26248,7 +26375,7 @@
         <v>896</v>
       </c>
       <c r="B882" t="s">
-        <v>896</v>
+        <v>17</v>
       </c>
       <c r="C882">
         <v>195</v>
@@ -26259,7 +26386,7 @@
         <v>897</v>
       </c>
       <c r="B883" t="s">
-        <v>897</v>
+        <v>43</v>
       </c>
       <c r="C883">
         <v>194</v>
@@ -26270,7 +26397,7 @@
         <v>898</v>
       </c>
       <c r="B884" t="s">
-        <v>898</v>
+        <v>5373</v>
       </c>
       <c r="C884">
         <v>194</v>
@@ -26292,7 +26419,7 @@
         <v>900</v>
       </c>
       <c r="B886" t="s">
-        <v>900</v>
+        <v>5317</v>
       </c>
       <c r="C886">
         <v>194</v>
@@ -26303,7 +26430,7 @@
         <v>901</v>
       </c>
       <c r="B887" t="s">
-        <v>901</v>
+        <v>5371</v>
       </c>
       <c r="C887">
         <v>194</v>
@@ -26314,7 +26441,7 @@
         <v>902</v>
       </c>
       <c r="B888" t="s">
-        <v>902</v>
+        <v>59</v>
       </c>
       <c r="C888">
         <v>193</v>
@@ -26336,7 +26463,7 @@
         <v>904</v>
       </c>
       <c r="B890" t="s">
-        <v>904</v>
+        <v>216</v>
       </c>
       <c r="C890">
         <v>191</v>
@@ -26347,7 +26474,7 @@
         <v>905</v>
       </c>
       <c r="B891" t="s">
-        <v>905</v>
+        <v>5374</v>
       </c>
       <c r="C891">
         <v>190</v>
@@ -26358,7 +26485,7 @@
         <v>906</v>
       </c>
       <c r="B892" t="s">
-        <v>906</v>
+        <v>5</v>
       </c>
       <c r="C892">
         <v>190</v>
@@ -26369,7 +26496,7 @@
         <v>907</v>
       </c>
       <c r="B893" t="s">
-        <v>907</v>
+        <v>5375</v>
       </c>
       <c r="C893">
         <v>190</v>
@@ -26380,7 +26507,7 @@
         <v>908</v>
       </c>
       <c r="B894" t="s">
-        <v>908</v>
+        <v>5</v>
       </c>
       <c r="C894">
         <v>190</v>
@@ -26391,7 +26518,7 @@
         <v>909</v>
       </c>
       <c r="B895" t="s">
-        <v>909</v>
+        <v>161</v>
       </c>
       <c r="C895">
         <v>188</v>
@@ -26413,7 +26540,7 @@
         <v>911</v>
       </c>
       <c r="B897" t="s">
-        <v>911</v>
+        <v>5376</v>
       </c>
       <c r="C897">
         <v>187</v>
@@ -26446,7 +26573,7 @@
         <v>914</v>
       </c>
       <c r="B900" t="s">
-        <v>914</v>
+        <v>532</v>
       </c>
       <c r="C900">
         <v>186</v>
@@ -26490,7 +26617,7 @@
         <v>918</v>
       </c>
       <c r="B904" t="s">
-        <v>918</v>
+        <v>185</v>
       </c>
       <c r="C904">
         <v>185</v>
@@ -26501,7 +26628,7 @@
         <v>919</v>
       </c>
       <c r="B905" t="s">
-        <v>919</v>
+        <v>90</v>
       </c>
       <c r="C905">
         <v>184</v>
@@ -26512,7 +26639,7 @@
         <v>920</v>
       </c>
       <c r="B906" t="s">
-        <v>920</v>
+        <v>344</v>
       </c>
       <c r="C906">
         <v>184</v>
@@ -26534,7 +26661,7 @@
         <v>922</v>
       </c>
       <c r="B908" t="s">
-        <v>922</v>
+        <v>5377</v>
       </c>
       <c r="C908">
         <v>184</v>
@@ -26545,7 +26672,7 @@
         <v>923</v>
       </c>
       <c r="B909" t="s">
-        <v>923</v>
+        <v>95</v>
       </c>
       <c r="C909">
         <v>184</v>
@@ -26556,7 +26683,7 @@
         <v>924</v>
       </c>
       <c r="B910" t="s">
-        <v>924</v>
+        <v>465</v>
       </c>
       <c r="C910">
         <v>183</v>
@@ -26600,7 +26727,7 @@
         <v>928</v>
       </c>
       <c r="B914" t="s">
-        <v>928</v>
+        <v>5378</v>
       </c>
       <c r="C914">
         <v>181</v>
@@ -26611,7 +26738,7 @@
         <v>929</v>
       </c>
       <c r="B915" t="s">
-        <v>929</v>
+        <v>203</v>
       </c>
       <c r="C915">
         <v>181</v>
@@ -26644,7 +26771,7 @@
         <v>932</v>
       </c>
       <c r="B918" t="s">
-        <v>932</v>
+        <v>1128</v>
       </c>
       <c r="C918">
         <v>181</v>
@@ -26655,7 +26782,7 @@
         <v>933</v>
       </c>
       <c r="B919" t="s">
-        <v>933</v>
+        <v>166</v>
       </c>
       <c r="C919">
         <v>181</v>
@@ -26666,7 +26793,7 @@
         <v>934</v>
       </c>
       <c r="B920" t="s">
-        <v>934</v>
+        <v>250</v>
       </c>
       <c r="C920">
         <v>180</v>
@@ -26677,7 +26804,7 @@
         <v>935</v>
       </c>
       <c r="B921" t="s">
-        <v>935</v>
+        <v>5379</v>
       </c>
       <c r="C921">
         <v>180</v>
@@ -26688,7 +26815,7 @@
         <v>936</v>
       </c>
       <c r="B922" t="s">
-        <v>936</v>
+        <v>5380</v>
       </c>
       <c r="C922">
         <v>180</v>
@@ -26699,7 +26826,7 @@
         <v>937</v>
       </c>
       <c r="B923" t="s">
-        <v>937</v>
+        <v>250</v>
       </c>
       <c r="C923">
         <v>180</v>
@@ -26710,7 +26837,7 @@
         <v>938</v>
       </c>
       <c r="B924" t="s">
-        <v>938</v>
+        <v>199</v>
       </c>
       <c r="C924">
         <v>179</v>
@@ -26721,7 +26848,7 @@
         <v>939</v>
       </c>
       <c r="B925" t="s">
-        <v>939</v>
+        <v>207</v>
       </c>
       <c r="C925">
         <v>178</v>
@@ -26743,7 +26870,7 @@
         <v>941</v>
       </c>
       <c r="B927" t="s">
-        <v>941</v>
+        <v>1193</v>
       </c>
       <c r="C927">
         <v>178</v>
@@ -26754,7 +26881,7 @@
         <v>942</v>
       </c>
       <c r="B928" t="s">
-        <v>942</v>
+        <v>5381</v>
       </c>
       <c r="C928">
         <v>177</v>
@@ -26765,7 +26892,7 @@
         <v>943</v>
       </c>
       <c r="B929" t="s">
-        <v>943</v>
+        <v>422</v>
       </c>
       <c r="C929">
         <v>177</v>
@@ -26776,7 +26903,7 @@
         <v>944</v>
       </c>
       <c r="B930" t="s">
-        <v>944</v>
+        <v>5332</v>
       </c>
       <c r="C930">
         <v>177</v>
@@ -26787,7 +26914,7 @@
         <v>945</v>
       </c>
       <c r="B931" t="s">
-        <v>945</v>
+        <v>222</v>
       </c>
       <c r="C931">
         <v>176</v>
@@ -26809,7 +26936,7 @@
         <v>947</v>
       </c>
       <c r="B933" t="s">
-        <v>947</v>
+        <v>555</v>
       </c>
       <c r="C933">
         <v>175</v>
@@ -26820,7 +26947,7 @@
         <v>948</v>
       </c>
       <c r="B934" t="s">
-        <v>948</v>
+        <v>989</v>
       </c>
       <c r="C934">
         <v>175</v>
@@ -26831,7 +26958,7 @@
         <v>949</v>
       </c>
       <c r="B935" t="s">
-        <v>949</v>
+        <v>5382</v>
       </c>
       <c r="C935">
         <v>175</v>
@@ -26842,7 +26969,7 @@
         <v>950</v>
       </c>
       <c r="B936" t="s">
-        <v>950</v>
+        <v>5383</v>
       </c>
       <c r="C936">
         <v>174</v>
@@ -26853,7 +26980,7 @@
         <v>951</v>
       </c>
       <c r="B937" t="s">
-        <v>951</v>
+        <v>893</v>
       </c>
       <c r="C937">
         <v>174</v>
@@ -26886,7 +27013,7 @@
         <v>954</v>
       </c>
       <c r="B940" t="s">
-        <v>954</v>
+        <v>725</v>
       </c>
       <c r="C940">
         <v>173</v>
@@ -26897,7 +27024,7 @@
         <v>955</v>
       </c>
       <c r="B941" t="s">
-        <v>955</v>
+        <v>773</v>
       </c>
       <c r="C941">
         <v>173</v>
@@ -26941,7 +27068,7 @@
         <v>959</v>
       </c>
       <c r="B945" t="s">
-        <v>959</v>
+        <v>5310</v>
       </c>
       <c r="C945">
         <v>171</v>
@@ -26974,7 +27101,7 @@
         <v>962</v>
       </c>
       <c r="B948" t="s">
-        <v>962</v>
+        <v>4</v>
       </c>
       <c r="C948">
         <v>170</v>
@@ -26985,7 +27112,7 @@
         <v>963</v>
       </c>
       <c r="B949" t="s">
-        <v>963</v>
+        <v>250</v>
       </c>
       <c r="C949">
         <v>170</v>
@@ -26996,7 +27123,7 @@
         <v>964</v>
       </c>
       <c r="B950" t="s">
-        <v>964</v>
+        <v>5384</v>
       </c>
       <c r="C950">
         <v>170</v>
@@ -27040,7 +27167,7 @@
         <v>968</v>
       </c>
       <c r="B954" t="s">
-        <v>968</v>
+        <v>487</v>
       </c>
       <c r="C954">
         <v>169</v>
@@ -27051,7 +27178,7 @@
         <v>969</v>
       </c>
       <c r="B955" t="s">
-        <v>969</v>
+        <v>276</v>
       </c>
       <c r="C955">
         <v>168</v>
@@ -27062,7 +27189,7 @@
         <v>970</v>
       </c>
       <c r="B956" t="s">
-        <v>970</v>
+        <v>192</v>
       </c>
       <c r="C956">
         <v>167</v>
@@ -27073,7 +27200,7 @@
         <v>971</v>
       </c>
       <c r="B957" t="s">
-        <v>971</v>
+        <v>250</v>
       </c>
       <c r="C957">
         <v>167</v>
@@ -27084,7 +27211,7 @@
         <v>972</v>
       </c>
       <c r="B958" t="s">
-        <v>972</v>
+        <v>178</v>
       </c>
       <c r="C958">
         <v>167</v>
@@ -27095,7 +27222,7 @@
         <v>973</v>
       </c>
       <c r="B959" t="s">
-        <v>973</v>
+        <v>5385</v>
       </c>
       <c r="C959">
         <v>167</v>
@@ -27106,7 +27233,7 @@
         <v>974</v>
       </c>
       <c r="B960" t="s">
-        <v>974</v>
+        <v>532</v>
       </c>
       <c r="C960">
         <v>166</v>
@@ -27117,7 +27244,7 @@
         <v>975</v>
       </c>
       <c r="B961" t="s">
-        <v>975</v>
+        <v>773</v>
       </c>
       <c r="C961">
         <v>166</v>
@@ -27139,7 +27266,7 @@
         <v>977</v>
       </c>
       <c r="B963" t="s">
-        <v>977</v>
+        <v>5386</v>
       </c>
       <c r="C963">
         <v>165</v>
@@ -27150,7 +27277,7 @@
         <v>978</v>
       </c>
       <c r="B964" t="s">
-        <v>978</v>
+        <v>364</v>
       </c>
       <c r="C964">
         <v>165</v>
@@ -27161,7 +27288,7 @@
         <v>979</v>
       </c>
       <c r="B965" t="s">
-        <v>979</v>
+        <v>396</v>
       </c>
       <c r="C965">
         <v>165</v>
@@ -27172,7 +27299,7 @@
         <v>980</v>
       </c>
       <c r="B966" t="s">
-        <v>980</v>
+        <v>5</v>
       </c>
       <c r="C966">
         <v>164</v>
@@ -27183,7 +27310,7 @@
         <v>981</v>
       </c>
       <c r="B967" t="s">
-        <v>981</v>
+        <v>208</v>
       </c>
       <c r="C967">
         <v>164</v>
@@ -27194,7 +27321,7 @@
         <v>982</v>
       </c>
       <c r="B968" t="s">
-        <v>982</v>
+        <v>5387</v>
       </c>
       <c r="C968">
         <v>164</v>
@@ -27205,7 +27332,7 @@
         <v>983</v>
       </c>
       <c r="B969" t="s">
-        <v>983</v>
+        <v>268</v>
       </c>
       <c r="C969">
         <v>163</v>
@@ -27216,7 +27343,7 @@
         <v>984</v>
       </c>
       <c r="B970" t="s">
-        <v>984</v>
+        <v>5328</v>
       </c>
       <c r="C970">
         <v>163</v>
@@ -27238,7 +27365,7 @@
         <v>986</v>
       </c>
       <c r="B972" t="s">
-        <v>986</v>
+        <v>1688</v>
       </c>
       <c r="C972">
         <v>163</v>
@@ -27249,7 +27376,7 @@
         <v>987</v>
       </c>
       <c r="B973" t="s">
-        <v>987</v>
+        <v>749</v>
       </c>
       <c r="C973">
         <v>163</v>
@@ -27260,7 +27387,7 @@
         <v>988</v>
       </c>
       <c r="B974" t="s">
-        <v>988</v>
+        <v>1303</v>
       </c>
       <c r="C974">
         <v>162</v>
@@ -27304,7 +27431,7 @@
         <v>992</v>
       </c>
       <c r="B978" t="s">
-        <v>992</v>
+        <v>706</v>
       </c>
       <c r="C978">
         <v>161</v>
@@ -27315,7 +27442,7 @@
         <v>993</v>
       </c>
       <c r="B979" t="s">
-        <v>993</v>
+        <v>191</v>
       </c>
       <c r="C979">
         <v>161</v>
@@ -27326,7 +27453,7 @@
         <v>994</v>
       </c>
       <c r="B980" t="s">
-        <v>994</v>
+        <v>295</v>
       </c>
       <c r="C980">
         <v>161</v>
@@ -27337,7 +27464,7 @@
         <v>995</v>
       </c>
       <c r="B981" t="s">
-        <v>995</v>
+        <v>74</v>
       </c>
       <c r="C981">
         <v>160</v>
@@ -27359,7 +27486,7 @@
         <v>997</v>
       </c>
       <c r="B983" t="s">
-        <v>997</v>
+        <v>505</v>
       </c>
       <c r="C983">
         <v>160</v>
@@ -27370,7 +27497,7 @@
         <v>998</v>
       </c>
       <c r="B984" t="s">
-        <v>998</v>
+        <v>185</v>
       </c>
       <c r="C984">
         <v>160</v>
@@ -27392,7 +27519,7 @@
         <v>1000</v>
       </c>
       <c r="B986" t="s">
-        <v>1000</v>
+        <v>344</v>
       </c>
       <c r="C986">
         <v>159</v>
@@ -27403,7 +27530,7 @@
         <v>1001</v>
       </c>
       <c r="B987" t="s">
-        <v>1001</v>
+        <v>187</v>
       </c>
       <c r="C987">
         <v>159</v>
@@ -27414,7 +27541,7 @@
         <v>1002</v>
       </c>
       <c r="B988" t="s">
-        <v>1002</v>
+        <v>53</v>
       </c>
       <c r="C988">
         <v>158</v>
@@ -27425,7 +27552,7 @@
         <v>1003</v>
       </c>
       <c r="B989" t="s">
-        <v>1003</v>
+        <v>5388</v>
       </c>
       <c r="C989">
         <v>158</v>
@@ -27436,7 +27563,7 @@
         <v>1004</v>
       </c>
       <c r="B990" t="s">
-        <v>1004</v>
+        <v>250</v>
       </c>
       <c r="C990">
         <v>158</v>
@@ -27458,7 +27585,7 @@
         <v>1006</v>
       </c>
       <c r="B992" t="s">
-        <v>1006</v>
+        <v>912</v>
       </c>
       <c r="C992">
         <v>157</v>
@@ -27480,7 +27607,7 @@
         <v>1008</v>
       </c>
       <c r="B994" t="s">
-        <v>1008</v>
+        <v>1259</v>
       </c>
       <c r="C994">
         <v>157</v>
@@ -27491,7 +27618,7 @@
         <v>1009</v>
       </c>
       <c r="B995" t="s">
-        <v>1009</v>
+        <v>5389</v>
       </c>
       <c r="C995">
         <v>156</v>
@@ -27502,7 +27629,7 @@
         <v>1010</v>
       </c>
       <c r="B996" t="s">
-        <v>1010</v>
+        <v>121</v>
       </c>
       <c r="C996">
         <v>156</v>
@@ -27513,7 +27640,7 @@
         <v>1011</v>
       </c>
       <c r="B997" t="s">
-        <v>1011</v>
+        <v>465</v>
       </c>
       <c r="C997">
         <v>156</v>
@@ -27524,7 +27651,7 @@
         <v>1012</v>
       </c>
       <c r="B998" t="s">
-        <v>1012</v>
+        <v>396</v>
       </c>
       <c r="C998">
         <v>156</v>
@@ -27535,7 +27662,7 @@
         <v>1013</v>
       </c>
       <c r="B999" t="s">
-        <v>1013</v>
+        <v>5390</v>
       </c>
       <c r="C999">
         <v>156</v>
@@ -27545,8 +27672,8 @@
       <c r="A1000" t="s">
         <v>1014</v>
       </c>
-      <c r="B1000" t="s">
-        <v>1014</v>
+      <c r="B1000" s="2" t="s">
+        <v>5391</v>
       </c>
       <c r="C1000">
         <v>155</v>
@@ -27557,7 +27684,7 @@
         <v>1015</v>
       </c>
       <c r="B1001" t="s">
-        <v>1015</v>
+        <v>78</v>
       </c>
       <c r="C1001">
         <v>154</v>
@@ -27590,7 +27717,7 @@
         <v>1019</v>
       </c>
       <c r="B1004" t="s">
-        <v>1019</v>
+        <v>4</v>
       </c>
       <c r="C1004">
         <v>152</v>
@@ -27601,7 +27728,7 @@
         <v>1020</v>
       </c>
       <c r="B1005" t="s">
-        <v>1020</v>
+        <v>5392</v>
       </c>
       <c r="C1005">
         <v>151</v>
@@ -27623,7 +27750,7 @@
         <v>1022</v>
       </c>
       <c r="B1007" t="s">
-        <v>1022</v>
+        <v>795</v>
       </c>
       <c r="C1007">
         <v>150</v>
@@ -27634,7 +27761,7 @@
         <v>1023</v>
       </c>
       <c r="B1008" t="s">
-        <v>1023</v>
+        <v>29</v>
       </c>
       <c r="C1008">
         <v>150</v>
@@ -27656,7 +27783,7 @@
         <v>1025</v>
       </c>
       <c r="B1010" t="s">
-        <v>1025</v>
+        <v>7</v>
       </c>
       <c r="C1010">
         <v>150</v>
@@ -27678,7 +27805,7 @@
         <v>1027</v>
       </c>
       <c r="B1012" t="s">
-        <v>1027</v>
+        <v>818</v>
       </c>
       <c r="C1012">
         <v>150</v>
@@ -27689,7 +27816,7 @@
         <v>1028</v>
       </c>
       <c r="B1013" t="s">
-        <v>1028</v>
+        <v>136</v>
       </c>
       <c r="C1013">
         <v>149</v>
@@ -27700,7 +27827,7 @@
         <v>1029</v>
       </c>
       <c r="B1014" t="s">
-        <v>1029</v>
+        <v>407</v>
       </c>
       <c r="C1014">
         <v>149</v>
@@ -27711,7 +27838,7 @@
         <v>1030</v>
       </c>
       <c r="B1015" t="s">
-        <v>1030</v>
+        <v>34</v>
       </c>
       <c r="C1015">
         <v>148</v>
@@ -27722,7 +27849,7 @@
         <v>1031</v>
       </c>
       <c r="B1016" t="s">
-        <v>1031</v>
+        <v>1994</v>
       </c>
       <c r="C1016">
         <v>148</v>
@@ -27744,7 +27871,7 @@
         <v>1034</v>
       </c>
       <c r="B1018" t="s">
-        <v>1034</v>
+        <v>1688</v>
       </c>
       <c r="C1018">
         <v>148</v>
@@ -27766,7 +27893,7 @@
         <v>1036</v>
       </c>
       <c r="B1020" t="s">
-        <v>1036</v>
+        <v>532</v>
       </c>
       <c r="C1020">
         <v>147</v>
@@ -27777,7 +27904,7 @@
         <v>1037</v>
       </c>
       <c r="B1021" t="s">
-        <v>1037</v>
+        <v>396</v>
       </c>
       <c r="C1021">
         <v>147</v>
@@ -27788,7 +27915,7 @@
         <v>1038</v>
       </c>
       <c r="B1022" t="s">
-        <v>1038</v>
+        <v>364</v>
       </c>
       <c r="C1022">
         <v>146</v>
@@ -27810,7 +27937,7 @@
         <v>1040</v>
       </c>
       <c r="B1024" t="s">
-        <v>1040</v>
+        <v>633</v>
       </c>
       <c r="C1024">
         <v>146</v>
@@ -27832,7 +27959,7 @@
         <v>1042</v>
       </c>
       <c r="B1026" t="s">
-        <v>1042</v>
+        <v>283</v>
       </c>
       <c r="C1026">
         <v>146</v>
@@ -27843,7 +27970,7 @@
         <v>1043</v>
       </c>
       <c r="B1027" t="s">
-        <v>1043</v>
+        <v>17</v>
       </c>
       <c r="C1027">
         <v>145</v>
@@ -27854,7 +27981,7 @@
         <v>1044</v>
       </c>
       <c r="B1028" t="s">
-        <v>1044</v>
+        <v>29</v>
       </c>
       <c r="C1028">
         <v>144</v>
@@ -27865,7 +27992,7 @@
         <v>1045</v>
       </c>
       <c r="B1029" t="s">
-        <v>1045</v>
+        <v>465</v>
       </c>
       <c r="C1029">
         <v>144</v>
@@ -27876,7 +28003,7 @@
         <v>1046</v>
       </c>
       <c r="B1030" t="s">
-        <v>1046</v>
+        <v>377</v>
       </c>
       <c r="C1030">
         <v>143</v>
@@ -27909,7 +28036,7 @@
         <v>1049</v>
       </c>
       <c r="B1033" t="s">
-        <v>1049</v>
+        <v>177</v>
       </c>
       <c r="C1033">
         <v>142</v>
@@ -27920,7 +28047,7 @@
         <v>1050</v>
       </c>
       <c r="B1034" t="s">
-        <v>1050</v>
+        <v>5393</v>
       </c>
       <c r="C1034">
         <v>142</v>
@@ -27931,7 +28058,7 @@
         <v>1051</v>
       </c>
       <c r="B1035" t="s">
-        <v>1051</v>
+        <v>5317</v>
       </c>
       <c r="C1035">
         <v>141</v>
@@ -27942,7 +28069,7 @@
         <v>1052</v>
       </c>
       <c r="B1036" t="s">
-        <v>1052</v>
+        <v>505</v>
       </c>
       <c r="C1036">
         <v>141</v>
@@ -27953,7 +28080,7 @@
         <v>1053</v>
       </c>
       <c r="B1037" t="s">
-        <v>1053</v>
+        <v>43</v>
       </c>
       <c r="C1037">
         <v>141</v>
@@ -27975,7 +28102,7 @@
         <v>1055</v>
       </c>
       <c r="B1039" t="s">
-        <v>1055</v>
+        <v>131</v>
       </c>
       <c r="C1039">
         <v>140</v>
@@ -27986,7 +28113,7 @@
         <v>1056</v>
       </c>
       <c r="B1040" t="s">
-        <v>1056</v>
+        <v>5371</v>
       </c>
       <c r="C1040">
         <v>140</v>
@@ -27997,7 +28124,7 @@
         <v>1057</v>
       </c>
       <c r="B1041" t="s">
-        <v>1057</v>
+        <v>33</v>
       </c>
       <c r="C1041">
         <v>140</v>
@@ -28008,7 +28135,7 @@
         <v>1058</v>
       </c>
       <c r="B1042" t="s">
-        <v>1058</v>
+        <v>478</v>
       </c>
       <c r="C1042">
         <v>140</v>
@@ -28019,7 +28146,7 @@
         <v>1059</v>
       </c>
       <c r="B1043" t="s">
-        <v>1059</v>
+        <v>5394</v>
       </c>
       <c r="C1043">
         <v>140</v>
@@ -28041,7 +28168,7 @@
         <v>1061</v>
       </c>
       <c r="B1045" t="s">
-        <v>1061</v>
+        <v>5395</v>
       </c>
       <c r="C1045">
         <v>139</v>
@@ -28052,7 +28179,7 @@
         <v>1062</v>
       </c>
       <c r="B1046" t="s">
-        <v>1062</v>
+        <v>5332</v>
       </c>
       <c r="C1046">
         <v>138</v>
@@ -28074,7 +28201,7 @@
         <v>1064</v>
       </c>
       <c r="B1048" t="s">
-        <v>1064</v>
+        <v>178</v>
       </c>
       <c r="C1048">
         <v>138</v>
@@ -28085,7 +28212,7 @@
         <v>1065</v>
       </c>
       <c r="B1049" t="s">
-        <v>1065</v>
+        <v>53</v>
       </c>
       <c r="C1049">
         <v>138</v>
@@ -28096,7 +28223,7 @@
         <v>1066</v>
       </c>
       <c r="B1050" t="s">
-        <v>1066</v>
+        <v>282</v>
       </c>
       <c r="C1050">
         <v>138</v>
@@ -28118,7 +28245,7 @@
         <v>1068</v>
       </c>
       <c r="B1052" t="s">
-        <v>1068</v>
+        <v>78</v>
       </c>
       <c r="C1052">
         <v>138</v>
@@ -28129,7 +28256,7 @@
         <v>1069</v>
       </c>
       <c r="B1053" t="s">
-        <v>1069</v>
+        <v>203</v>
       </c>
       <c r="C1053">
         <v>138</v>
@@ -28140,7 +28267,7 @@
         <v>1070</v>
       </c>
       <c r="B1054" t="s">
-        <v>1070</v>
+        <v>1540</v>
       </c>
       <c r="C1054">
         <v>137</v>
@@ -28151,7 +28278,7 @@
         <v>1071</v>
       </c>
       <c r="B1055" t="s">
-        <v>1071</v>
+        <v>749</v>
       </c>
       <c r="C1055">
         <v>137</v>
@@ -28173,7 +28300,7 @@
         <v>1073</v>
       </c>
       <c r="B1057" t="s">
-        <v>1073</v>
+        <v>736</v>
       </c>
       <c r="C1057">
         <v>137</v>
@@ -28195,7 +28322,7 @@
         <v>1076</v>
       </c>
       <c r="B1059" t="s">
-        <v>1076</v>
+        <v>415</v>
       </c>
       <c r="C1059">
         <v>136</v>
@@ -28206,7 +28333,7 @@
         <v>1077</v>
       </c>
       <c r="B1060" t="s">
-        <v>1077</v>
+        <v>5337</v>
       </c>
       <c r="C1060">
         <v>136</v>
@@ -28217,7 +28344,7 @@
         <v>1078</v>
       </c>
       <c r="B1061" t="s">
-        <v>1078</v>
+        <v>121</v>
       </c>
       <c r="C1061">
         <v>136</v>
@@ -28239,7 +28366,7 @@
         <v>1080</v>
       </c>
       <c r="B1063" t="s">
-        <v>1080</v>
+        <v>57</v>
       </c>
       <c r="C1063">
         <v>136</v>
@@ -28261,7 +28388,7 @@
         <v>1082</v>
       </c>
       <c r="B1065" t="s">
-        <v>1082</v>
+        <v>5396</v>
       </c>
       <c r="C1065">
         <v>135</v>
@@ -28272,7 +28399,7 @@
         <v>1083</v>
       </c>
       <c r="B1066" t="s">
-        <v>1083</v>
+        <v>136</v>
       </c>
       <c r="C1066">
         <v>134</v>
@@ -28283,7 +28410,7 @@
         <v>1084</v>
       </c>
       <c r="B1067" t="s">
-        <v>1084</v>
+        <v>516</v>
       </c>
       <c r="C1067">
         <v>134</v>
@@ -28294,7 +28421,7 @@
         <v>1085</v>
       </c>
       <c r="B1068" t="s">
-        <v>1085</v>
+        <v>465</v>
       </c>
       <c r="C1068">
         <v>134</v>
@@ -28305,7 +28432,7 @@
         <v>1086</v>
       </c>
       <c r="B1069" t="s">
-        <v>1086</v>
+        <v>203</v>
       </c>
       <c r="C1069">
         <v>133</v>
@@ -28316,7 +28443,7 @@
         <v>1087</v>
       </c>
       <c r="B1070" t="s">
-        <v>1087</v>
+        <v>10</v>
       </c>
       <c r="C1070">
         <v>133</v>
@@ -28327,7 +28454,7 @@
         <v>1088</v>
       </c>
       <c r="B1071" t="s">
-        <v>1088</v>
+        <v>725</v>
       </c>
       <c r="C1071">
         <v>133</v>
@@ -28338,7 +28465,7 @@
         <v>1089</v>
       </c>
       <c r="B1072" t="s">
-        <v>1089</v>
+        <v>1485</v>
       </c>
       <c r="C1072">
         <v>132</v>
@@ -28349,7 +28476,7 @@
         <v>1090</v>
       </c>
       <c r="B1073" t="s">
-        <v>1090</v>
+        <v>850</v>
       </c>
       <c r="C1073">
         <v>131</v>
@@ -28360,7 +28487,7 @@
         <v>1091</v>
       </c>
       <c r="B1074" t="s">
-        <v>1091</v>
+        <v>532</v>
       </c>
       <c r="C1074">
         <v>131</v>
@@ -28382,7 +28509,7 @@
         <v>1093</v>
       </c>
       <c r="B1076" t="s">
-        <v>1093</v>
+        <v>136</v>
       </c>
       <c r="C1076">
         <v>131</v>
@@ -28404,7 +28531,7 @@
         <v>1095</v>
       </c>
       <c r="B1078" t="s">
-        <v>1095</v>
+        <v>725</v>
       </c>
       <c r="C1078">
         <v>131</v>
@@ -28415,7 +28542,7 @@
         <v>1096</v>
       </c>
       <c r="B1079" t="s">
-        <v>1096</v>
+        <v>637</v>
       </c>
       <c r="C1079">
         <v>131</v>
@@ -28426,7 +28553,7 @@
         <v>1097</v>
       </c>
       <c r="B1080" t="s">
-        <v>1097</v>
+        <v>161</v>
       </c>
       <c r="C1080">
         <v>130</v>
@@ -28437,7 +28564,7 @@
         <v>1098</v>
       </c>
       <c r="B1081" t="s">
-        <v>1098</v>
+        <v>175</v>
       </c>
       <c r="C1081">
         <v>130</v>
@@ -28448,7 +28575,7 @@
         <v>1099</v>
       </c>
       <c r="B1082" t="s">
-        <v>1099</v>
+        <v>11</v>
       </c>
       <c r="C1082">
         <v>130</v>
@@ -28459,7 +28586,7 @@
         <v>1100</v>
       </c>
       <c r="B1083" t="s">
-        <v>1100</v>
+        <v>465</v>
       </c>
       <c r="C1083">
         <v>130</v>
@@ -28470,7 +28597,7 @@
         <v>1101</v>
       </c>
       <c r="B1084" t="s">
-        <v>1101</v>
+        <v>396</v>
       </c>
       <c r="C1084">
         <v>130</v>
@@ -28481,7 +28608,7 @@
         <v>1102</v>
       </c>
       <c r="B1085" t="s">
-        <v>1102</v>
+        <v>3054</v>
       </c>
       <c r="C1085">
         <v>129</v>
@@ -28492,7 +28619,7 @@
         <v>1103</v>
       </c>
       <c r="B1086" t="s">
-        <v>1103</v>
+        <v>279</v>
       </c>
       <c r="C1086">
         <v>129</v>
@@ -28514,7 +28641,7 @@
         <v>1105</v>
       </c>
       <c r="B1088" t="s">
-        <v>1105</v>
+        <v>136</v>
       </c>
       <c r="C1088">
         <v>128</v>
@@ -28536,7 +28663,7 @@
         <v>1107</v>
       </c>
       <c r="B1090" t="s">
-        <v>1107</v>
+        <v>9</v>
       </c>
       <c r="C1090">
         <v>128</v>
@@ -28547,7 +28674,7 @@
         <v>1108</v>
       </c>
       <c r="B1091" t="s">
-        <v>1108</v>
+        <v>5318</v>
       </c>
       <c r="C1091">
         <v>128</v>
@@ -28558,7 +28685,7 @@
         <v>1109</v>
       </c>
       <c r="B1092" t="s">
-        <v>1109</v>
+        <v>465</v>
       </c>
       <c r="C1092">
         <v>128</v>
@@ -28569,7 +28696,7 @@
         <v>1110</v>
       </c>
       <c r="B1093" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C1093">
         <v>127</v>
@@ -28580,7 +28707,7 @@
         <v>1111</v>
       </c>
       <c r="B1094" t="s">
-        <v>1111</v>
+        <v>41</v>
       </c>
       <c r="C1094">
         <v>127</v>
@@ -28591,7 +28718,7 @@
         <v>1112</v>
       </c>
       <c r="B1095" t="s">
-        <v>1112</v>
+        <v>222</v>
       </c>
       <c r="C1095">
         <v>127</v>
@@ -28613,7 +28740,7 @@
         <v>1114</v>
       </c>
       <c r="B1097" t="s">
-        <v>1114</v>
+        <v>3956</v>
       </c>
       <c r="C1097">
         <v>126</v>
@@ -28624,7 +28751,7 @@
         <v>1115</v>
       </c>
       <c r="B1098" t="s">
-        <v>1115</v>
+        <v>276</v>
       </c>
       <c r="C1098">
         <v>126</v>
@@ -28646,7 +28773,7 @@
         <v>1117</v>
       </c>
       <c r="B1100" t="s">
-        <v>1117</v>
+        <v>156</v>
       </c>
       <c r="C1100">
         <v>126</v>
@@ -28668,7 +28795,7 @@
         <v>1120</v>
       </c>
       <c r="B1102" t="s">
-        <v>1120</v>
+        <v>143</v>
       </c>
       <c r="C1102">
         <v>125</v>
@@ -28690,7 +28817,7 @@
         <v>1122</v>
       </c>
       <c r="B1104" t="s">
-        <v>1122</v>
+        <v>725</v>
       </c>
       <c r="C1104">
         <v>125</v>
@@ -28701,7 +28828,7 @@
         <v>1123</v>
       </c>
       <c r="B1105" t="s">
-        <v>1123</v>
+        <v>5397</v>
       </c>
       <c r="C1105">
         <v>125</v>
@@ -28712,7 +28839,7 @@
         <v>1124</v>
       </c>
       <c r="B1106" t="s">
-        <v>1124</v>
+        <v>5</v>
       </c>
       <c r="C1106">
         <v>125</v>
@@ -28723,7 +28850,7 @@
         <v>1125</v>
       </c>
       <c r="B1107" t="s">
-        <v>1125</v>
+        <v>532</v>
       </c>
       <c r="C1107">
         <v>125</v>
@@ -28734,7 +28861,7 @@
         <v>1126</v>
       </c>
       <c r="B1108" t="s">
-        <v>1126</v>
+        <v>5398</v>
       </c>
       <c r="C1108">
         <v>125</v>
@@ -28745,7 +28872,7 @@
         <v>1127</v>
       </c>
       <c r="B1109" t="s">
-        <v>1127</v>
+        <v>22</v>
       </c>
       <c r="C1109">
         <v>125</v>
@@ -28767,7 +28894,7 @@
         <v>1129</v>
       </c>
       <c r="B1111" t="s">
-        <v>1129</v>
+        <v>885</v>
       </c>
       <c r="C1111">
         <v>125</v>
@@ -28778,7 +28905,7 @@
         <v>1130</v>
       </c>
       <c r="B1112" t="s">
-        <v>1130</v>
+        <v>250</v>
       </c>
       <c r="C1112">
         <v>125</v>
@@ -28789,7 +28916,7 @@
         <v>1131</v>
       </c>
       <c r="B1113" t="s">
-        <v>1131</v>
+        <v>1423</v>
       </c>
       <c r="C1113">
         <v>124</v>
@@ -28800,7 +28927,7 @@
         <v>1132</v>
       </c>
       <c r="B1114" t="s">
-        <v>1132</v>
+        <v>5399</v>
       </c>
       <c r="C1114">
         <v>124</v>
@@ -28833,7 +28960,7 @@
         <v>1135</v>
       </c>
       <c r="B1117" t="s">
-        <v>1135</v>
+        <v>344</v>
       </c>
       <c r="C1117">
         <v>123</v>
@@ -28844,7 +28971,7 @@
         <v>1136</v>
       </c>
       <c r="B1118" t="s">
-        <v>1136</v>
+        <v>127</v>
       </c>
       <c r="C1118">
         <v>123</v>
@@ -28855,7 +28982,7 @@
         <v>1137</v>
       </c>
       <c r="B1119" t="s">
-        <v>1137</v>
+        <v>494</v>
       </c>
       <c r="C1119">
         <v>122</v>
@@ -28866,7 +28993,7 @@
         <v>1138</v>
       </c>
       <c r="B1120" t="s">
-        <v>1138</v>
+        <v>11</v>
       </c>
       <c r="C1120">
         <v>122</v>
@@ -28877,7 +29004,7 @@
         <v>1139</v>
       </c>
       <c r="B1121" t="s">
-        <v>1139</v>
+        <v>7</v>
       </c>
       <c r="C1121">
         <v>122</v>
@@ -28888,7 +29015,7 @@
         <v>1140</v>
       </c>
       <c r="B1122" t="s">
-        <v>1140</v>
+        <v>222</v>
       </c>
       <c r="C1122">
         <v>122</v>
@@ -28899,7 +29026,7 @@
         <v>1141</v>
       </c>
       <c r="B1123" t="s">
-        <v>1141</v>
+        <v>93</v>
       </c>
       <c r="C1123">
         <v>122</v>
@@ -28910,7 +29037,7 @@
         <v>1142</v>
       </c>
       <c r="B1124" t="s">
-        <v>1142</v>
+        <v>12</v>
       </c>
       <c r="C1124">
         <v>122</v>
@@ -28921,7 +29048,7 @@
         <v>1143</v>
       </c>
       <c r="B1125" t="s">
-        <v>1143</v>
+        <v>915</v>
       </c>
       <c r="C1125">
         <v>122</v>
@@ -28932,7 +29059,7 @@
         <v>1144</v>
       </c>
       <c r="B1126" t="s">
-        <v>1144</v>
+        <v>17</v>
       </c>
       <c r="C1126">
         <v>121</v>
@@ -28954,7 +29081,7 @@
         <v>1146</v>
       </c>
       <c r="B1128" t="s">
-        <v>1146</v>
+        <v>5400</v>
       </c>
       <c r="C1128">
         <v>121</v>
@@ -28965,7 +29092,7 @@
         <v>1147</v>
       </c>
       <c r="B1129" t="s">
-        <v>1147</v>
+        <v>185</v>
       </c>
       <c r="C1129">
         <v>121</v>
@@ -28987,7 +29114,7 @@
         <v>1149</v>
       </c>
       <c r="B1131" t="s">
-        <v>1149</v>
+        <v>11</v>
       </c>
       <c r="C1131">
         <v>120</v>
@@ -28998,7 +29125,7 @@
         <v>1150</v>
       </c>
       <c r="B1132" t="s">
-        <v>1150</v>
+        <v>364</v>
       </c>
       <c r="C1132">
         <v>120</v>
@@ -29009,7 +29136,7 @@
         <v>1151</v>
       </c>
       <c r="B1133" t="s">
-        <v>1151</v>
+        <v>364</v>
       </c>
       <c r="C1133">
         <v>120</v>
@@ -29031,7 +29158,7 @@
         <v>1153</v>
       </c>
       <c r="B1135" t="s">
-        <v>1153</v>
+        <v>516</v>
       </c>
       <c r="C1135">
         <v>119</v>
@@ -29042,7 +29169,7 @@
         <v>1154</v>
       </c>
       <c r="B1136" t="s">
-        <v>1154</v>
+        <v>487</v>
       </c>
       <c r="C1136">
         <v>119</v>
@@ -29053,7 +29180,7 @@
         <v>1155</v>
       </c>
       <c r="B1137" t="s">
-        <v>1155</v>
+        <v>4</v>
       </c>
       <c r="C1137">
         <v>119</v>
@@ -29064,7 +29191,7 @@
         <v>1156</v>
       </c>
       <c r="B1138" t="s">
-        <v>1156</v>
+        <v>5401</v>
       </c>
       <c r="C1138">
         <v>119</v>
@@ -29086,7 +29213,7 @@
         <v>1158</v>
       </c>
       <c r="B1140" t="s">
-        <v>1158</v>
+        <v>122</v>
       </c>
       <c r="C1140">
         <v>119</v>
@@ -29097,7 +29224,7 @@
         <v>1159</v>
       </c>
       <c r="B1141" t="s">
-        <v>1159</v>
+        <v>151</v>
       </c>
       <c r="C1141">
         <v>119</v>
@@ -29108,7 +29235,7 @@
         <v>1160</v>
       </c>
       <c r="B1142" t="s">
-        <v>1160</v>
+        <v>5375</v>
       </c>
       <c r="C1142">
         <v>118</v>
@@ -29130,7 +29257,7 @@
         <v>1162</v>
       </c>
       <c r="B1144" t="s">
-        <v>1162</v>
+        <v>192</v>
       </c>
       <c r="C1144">
         <v>118</v>
@@ -29141,7 +29268,7 @@
         <v>1163</v>
       </c>
       <c r="B1145" t="s">
-        <v>1163</v>
+        <v>364</v>
       </c>
       <c r="C1145">
         <v>118</v>
@@ -29152,7 +29279,7 @@
         <v>1164</v>
       </c>
       <c r="B1146" t="s">
-        <v>1164</v>
+        <v>5</v>
       </c>
       <c r="C1146">
         <v>118</v>
@@ -29163,7 +29290,7 @@
         <v>1165</v>
       </c>
       <c r="B1147" t="s">
-        <v>1165</v>
+        <v>178</v>
       </c>
       <c r="C1147">
         <v>118</v>
@@ -29174,7 +29301,7 @@
         <v>1166</v>
       </c>
       <c r="B1148" t="s">
-        <v>1166</v>
+        <v>83</v>
       </c>
       <c r="C1148">
         <v>118</v>
@@ -29185,7 +29312,7 @@
         <v>1167</v>
       </c>
       <c r="B1149" t="s">
-        <v>1168</v>
+        <v>116</v>
       </c>
       <c r="C1149">
         <v>117</v>
@@ -29207,7 +29334,7 @@
         <v>1170</v>
       </c>
       <c r="B1151" t="s">
-        <v>1170</v>
+        <v>49</v>
       </c>
       <c r="C1151">
         <v>117</v>
@@ -29218,7 +29345,7 @@
         <v>1171</v>
       </c>
       <c r="B1152" t="s">
-        <v>1171</v>
+        <v>465</v>
       </c>
       <c r="C1152">
         <v>117</v>
@@ -29240,7 +29367,7 @@
         <v>1173</v>
       </c>
       <c r="B1154" t="s">
-        <v>1173</v>
+        <v>250</v>
       </c>
       <c r="C1154">
         <v>117</v>
@@ -29251,7 +29378,7 @@
         <v>1174</v>
       </c>
       <c r="B1155" t="s">
-        <v>1174</v>
+        <v>5402</v>
       </c>
       <c r="C1155">
         <v>116</v>
@@ -29262,7 +29389,7 @@
         <v>1175</v>
       </c>
       <c r="B1156" t="s">
-        <v>1175</v>
+        <v>177</v>
       </c>
       <c r="C1156">
         <v>116</v>
@@ -29273,7 +29400,7 @@
         <v>1176</v>
       </c>
       <c r="B1157" t="s">
-        <v>1176</v>
+        <v>178</v>
       </c>
       <c r="C1157">
         <v>115</v>
@@ -29284,7 +29411,7 @@
         <v>1177</v>
       </c>
       <c r="B1158" t="s">
-        <v>1177</v>
+        <v>7</v>
       </c>
       <c r="C1158">
         <v>115</v>
@@ -29295,7 +29422,7 @@
         <v>1178</v>
       </c>
       <c r="B1159" t="s">
-        <v>1178</v>
+        <v>178</v>
       </c>
       <c r="C1159">
         <v>115</v>
@@ -29306,7 +29433,7 @@
         <v>1179</v>
       </c>
       <c r="B1160" t="s">
-        <v>1179</v>
+        <v>127</v>
       </c>
       <c r="C1160">
         <v>115</v>
@@ -29317,7 +29444,7 @@
         <v>1180</v>
       </c>
       <c r="B1161" t="s">
-        <v>1180</v>
+        <v>127</v>
       </c>
       <c r="C1161">
         <v>115</v>
@@ -29328,7 +29455,7 @@
         <v>1181</v>
       </c>
       <c r="B1162" t="s">
-        <v>1181</v>
+        <v>212</v>
       </c>
       <c r="C1162">
         <v>114</v>
@@ -29339,7 +29466,7 @@
         <v>1182</v>
       </c>
       <c r="B1163" t="s">
-        <v>1182</v>
+        <v>332</v>
       </c>
       <c r="C1163">
         <v>114</v>
@@ -29361,7 +29488,7 @@
         <v>1184</v>
       </c>
       <c r="B1165" t="s">
-        <v>1184</v>
+        <v>11</v>
       </c>
       <c r="C1165">
         <v>114</v>
@@ -29372,7 +29499,7 @@
         <v>1185</v>
       </c>
       <c r="B1166" t="s">
-        <v>1185</v>
+        <v>310</v>
       </c>
       <c r="C1166">
         <v>114</v>
@@ -29383,7 +29510,7 @@
         <v>1186</v>
       </c>
       <c r="B1167" t="s">
-        <v>1186</v>
+        <v>915</v>
       </c>
       <c r="C1167">
         <v>114</v>
@@ -29394,7 +29521,7 @@
         <v>1187</v>
       </c>
       <c r="B1168" t="s">
-        <v>1187</v>
+        <v>191</v>
       </c>
       <c r="C1168">
         <v>114</v>
@@ -29427,7 +29554,7 @@
         <v>1189</v>
       </c>
       <c r="B1171" t="s">
-        <v>1189</v>
+        <v>927</v>
       </c>
       <c r="C1171">
         <v>112</v>
@@ -29438,7 +29565,7 @@
         <v>1190</v>
       </c>
       <c r="B1172" t="s">
-        <v>1190</v>
+        <v>52</v>
       </c>
       <c r="C1172">
         <v>112</v>
@@ -29449,7 +29576,7 @@
         <v>1191</v>
       </c>
       <c r="B1173" t="s">
-        <v>1191</v>
+        <v>189</v>
       </c>
       <c r="C1173">
         <v>112</v>
@@ -29460,7 +29587,7 @@
         <v>1192</v>
       </c>
       <c r="B1174" t="s">
-        <v>1192</v>
+        <v>5345</v>
       </c>
       <c r="C1174">
         <v>112</v>
@@ -29482,7 +29609,7 @@
         <v>1194</v>
       </c>
       <c r="B1176" t="s">
-        <v>1194</v>
+        <v>250</v>
       </c>
       <c r="C1176">
         <v>111</v>
@@ -29493,7 +29620,7 @@
         <v>1195</v>
       </c>
       <c r="B1177" t="s">
-        <v>1195</v>
+        <v>5403</v>
       </c>
       <c r="C1177">
         <v>111</v>
@@ -29504,7 +29631,7 @@
         <v>1196</v>
       </c>
       <c r="B1178" t="s">
-        <v>1196</v>
+        <v>17</v>
       </c>
       <c r="C1178">
         <v>111</v>
@@ -29515,7 +29642,7 @@
         <v>1197</v>
       </c>
       <c r="B1179" t="s">
-        <v>1197</v>
+        <v>243</v>
       </c>
       <c r="C1179">
         <v>111</v>
@@ -29526,7 +29653,7 @@
         <v>1198</v>
       </c>
       <c r="B1180" t="s">
-        <v>1198</v>
+        <v>516</v>
       </c>
       <c r="C1180">
         <v>110</v>
@@ -29537,7 +29664,7 @@
         <v>1199</v>
       </c>
       <c r="B1181" t="s">
-        <v>1199</v>
+        <v>5404</v>
       </c>
       <c r="C1181">
         <v>110</v>
@@ -29548,7 +29675,7 @@
         <v>1200</v>
       </c>
       <c r="B1182" t="s">
-        <v>1200</v>
+        <v>22</v>
       </c>
       <c r="C1182">
         <v>110</v>
@@ -29559,7 +29686,7 @@
         <v>1201</v>
       </c>
       <c r="B1183" t="s">
-        <v>1201</v>
+        <v>692</v>
       </c>
       <c r="C1183">
         <v>110</v>
@@ -29570,7 +29697,7 @@
         <v>1202</v>
       </c>
       <c r="B1184" t="s">
-        <v>1202</v>
+        <v>120</v>
       </c>
       <c r="C1184">
         <v>109</v>
@@ -29581,7 +29708,7 @@
         <v>1203</v>
       </c>
       <c r="B1185" t="s">
-        <v>1203</v>
+        <v>811</v>
       </c>
       <c r="C1185">
         <v>109</v>
@@ -29592,7 +29719,7 @@
         <v>1204</v>
       </c>
       <c r="B1186" t="s">
-        <v>1204</v>
+        <v>207</v>
       </c>
       <c r="C1186">
         <v>109</v>
@@ -29603,7 +29730,7 @@
         <v>1205</v>
       </c>
       <c r="B1187" t="s">
-        <v>1205</v>
+        <v>227</v>
       </c>
       <c r="C1187">
         <v>109</v>
@@ -29614,7 +29741,7 @@
         <v>1206</v>
       </c>
       <c r="B1188" t="s">
-        <v>1206</v>
+        <v>5</v>
       </c>
       <c r="C1188">
         <v>109</v>
@@ -29636,7 +29763,7 @@
         <v>1208</v>
       </c>
       <c r="B1190" t="s">
-        <v>1208</v>
+        <v>211</v>
       </c>
       <c r="C1190">
         <v>108</v>
@@ -29647,7 +29774,7 @@
         <v>1209</v>
       </c>
       <c r="B1191" t="s">
-        <v>1209</v>
+        <v>187</v>
       </c>
       <c r="C1191">
         <v>108</v>
@@ -29669,7 +29796,7 @@
         <v>1211</v>
       </c>
       <c r="B1193" t="s">
-        <v>1211</v>
+        <v>364</v>
       </c>
       <c r="C1193">
         <v>108</v>
@@ -29691,7 +29818,7 @@
         <v>1213</v>
       </c>
       <c r="B1195" t="s">
-        <v>1213</v>
+        <v>57</v>
       </c>
       <c r="C1195">
         <v>107</v>
@@ -29702,7 +29829,7 @@
         <v>1214</v>
       </c>
       <c r="B1196" t="s">
-        <v>1214</v>
+        <v>250</v>
       </c>
       <c r="C1196">
         <v>107</v>
@@ -29713,7 +29840,7 @@
         <v>1215</v>
       </c>
       <c r="B1197" t="s">
-        <v>1215</v>
+        <v>5371</v>
       </c>
       <c r="C1197">
         <v>107</v>
@@ -29735,7 +29862,7 @@
         <v>1217</v>
       </c>
       <c r="B1199" t="s">
-        <v>1217</v>
+        <v>706</v>
       </c>
       <c r="C1199">
         <v>107</v>
@@ -29746,7 +29873,7 @@
         <v>1218</v>
       </c>
       <c r="B1200" t="s">
-        <v>1218</v>
+        <v>191</v>
       </c>
       <c r="C1200">
         <v>106</v>
@@ -29757,7 +29884,7 @@
         <v>1219</v>
       </c>
       <c r="B1201" t="s">
-        <v>1219</v>
+        <v>5405</v>
       </c>
       <c r="C1201">
         <v>106</v>
@@ -29768,7 +29895,7 @@
         <v>1220</v>
       </c>
       <c r="B1202" t="s">
-        <v>1220</v>
+        <v>250</v>
       </c>
       <c r="C1202">
         <v>106</v>
@@ -29779,7 +29906,7 @@
         <v>1221</v>
       </c>
       <c r="B1203" t="s">
-        <v>1221</v>
+        <v>364</v>
       </c>
       <c r="C1203">
         <v>106</v>
@@ -29790,7 +29917,7 @@
         <v>1222</v>
       </c>
       <c r="B1204" t="s">
-        <v>1222</v>
+        <v>364</v>
       </c>
       <c r="C1204">
         <v>105</v>
@@ -29801,7 +29928,7 @@
         <v>1223</v>
       </c>
       <c r="B1205" t="s">
-        <v>1223</v>
+        <v>532</v>
       </c>
       <c r="C1205">
         <v>105</v>
@@ -29812,7 +29939,7 @@
         <v>1224</v>
       </c>
       <c r="B1206" t="s">
-        <v>1224</v>
+        <v>295</v>
       </c>
       <c r="C1206">
         <v>105</v>
@@ -29823,7 +29950,7 @@
         <v>1225</v>
       </c>
       <c r="B1207" t="s">
-        <v>1225</v>
+        <v>930</v>
       </c>
       <c r="C1207">
         <v>105</v>
@@ -29834,7 +29961,7 @@
         <v>1226</v>
       </c>
       <c r="B1208" t="s">
-        <v>1226</v>
+        <v>203</v>
       </c>
       <c r="C1208">
         <v>105</v>
@@ -29845,7 +29972,7 @@
         <v>1227</v>
       </c>
       <c r="B1209" t="s">
-        <v>1227</v>
+        <v>189</v>
       </c>
       <c r="C1209">
         <v>105</v>
@@ -29878,7 +30005,7 @@
         <v>1230</v>
       </c>
       <c r="B1212" t="s">
-        <v>1230</v>
+        <v>307</v>
       </c>
       <c r="C1212">
         <v>104</v>
@@ -29900,7 +30027,7 @@
         <v>1232</v>
       </c>
       <c r="B1214" t="s">
-        <v>1232</v>
+        <v>335</v>
       </c>
       <c r="C1214">
         <v>104</v>
@@ -29911,7 +30038,7 @@
         <v>1233</v>
       </c>
       <c r="B1215" t="s">
-        <v>1233</v>
+        <v>5406</v>
       </c>
       <c r="C1215">
         <v>104</v>
@@ -29922,7 +30049,7 @@
         <v>1234</v>
       </c>
       <c r="B1216" t="s">
-        <v>1234</v>
+        <v>178</v>
       </c>
       <c r="C1216">
         <v>104</v>
@@ -29933,7 +30060,7 @@
         <v>1235</v>
       </c>
       <c r="B1217" t="s">
-        <v>1235</v>
+        <v>59</v>
       </c>
       <c r="C1217">
         <v>103</v>
@@ -29944,7 +30071,7 @@
         <v>1236</v>
       </c>
       <c r="B1218" t="s">
-        <v>1236</v>
+        <v>136</v>
       </c>
       <c r="C1218">
         <v>103</v>
@@ -29955,7 +30082,7 @@
         <v>1237</v>
       </c>
       <c r="B1219" t="s">
-        <v>1237</v>
+        <v>5407</v>
       </c>
       <c r="C1219">
         <v>103</v>
@@ -29966,7 +30093,7 @@
         <v>1238</v>
       </c>
       <c r="B1220" t="s">
-        <v>1238</v>
+        <v>177</v>
       </c>
       <c r="C1220">
         <v>103</v>
@@ -29977,7 +30104,7 @@
         <v>1239</v>
       </c>
       <c r="B1221" t="s">
-        <v>1239</v>
+        <v>68</v>
       </c>
       <c r="C1221">
         <v>102</v>
@@ -29988,7 +30115,7 @@
         <v>1240</v>
       </c>
       <c r="B1222" t="s">
-        <v>1240</v>
+        <v>5408</v>
       </c>
       <c r="C1222">
         <v>102</v>
@@ -29999,7 +30126,7 @@
         <v>1241</v>
       </c>
       <c r="B1223" t="s">
-        <v>1241</v>
+        <v>421</v>
       </c>
       <c r="C1223">
         <v>102</v>
@@ -30021,7 +30148,7 @@
         <v>1243</v>
       </c>
       <c r="B1225" t="s">
-        <v>1243</v>
+        <v>178</v>
       </c>
       <c r="C1225">
         <v>102</v>
@@ -30032,7 +30159,7 @@
         <v>1244</v>
       </c>
       <c r="B1226" t="s">
-        <v>1244</v>
+        <v>5318</v>
       </c>
       <c r="C1226">
         <v>102</v>
@@ -30043,7 +30170,7 @@
         <v>1245</v>
       </c>
       <c r="B1227" t="s">
-        <v>1245</v>
+        <v>141</v>
       </c>
       <c r="C1227">
         <v>102</v>
@@ -30054,7 +30181,7 @@
         <v>1246</v>
       </c>
       <c r="B1228" t="s">
-        <v>1247</v>
+        <v>479</v>
       </c>
       <c r="C1228">
         <v>101</v>
@@ -30065,7 +30192,7 @@
         <v>1248</v>
       </c>
       <c r="B1229" t="s">
-        <v>1248</v>
+        <v>5409</v>
       </c>
       <c r="C1229">
         <v>101</v>
@@ -30087,7 +30214,7 @@
         <v>1250</v>
       </c>
       <c r="B1231" t="s">
-        <v>1250</v>
+        <v>5410</v>
       </c>
       <c r="C1231">
         <v>101</v>
@@ -30098,7 +30225,7 @@
         <v>1251</v>
       </c>
       <c r="B1232" t="s">
-        <v>1251</v>
+        <v>1423</v>
       </c>
       <c r="C1232">
         <v>100</v>
@@ -30109,7 +30236,7 @@
         <v>1252</v>
       </c>
       <c r="B1233" t="s">
-        <v>1252</v>
+        <v>364</v>
       </c>
       <c r="C1233">
         <v>100</v>
@@ -30120,7 +30247,7 @@
         <v>1253</v>
       </c>
       <c r="B1234" t="s">
-        <v>1253</v>
+        <v>30</v>
       </c>
       <c r="C1234">
         <v>100</v>
@@ -30131,7 +30258,7 @@
         <v>1254</v>
       </c>
       <c r="B1235" t="s">
-        <v>1254</v>
+        <v>5411</v>
       </c>
       <c r="C1235">
         <v>100</v>
@@ -30142,7 +30269,7 @@
         <v>1255</v>
       </c>
       <c r="B1236" t="s">
-        <v>1255</v>
+        <v>465</v>
       </c>
       <c r="C1236">
         <v>100</v>
@@ -30153,7 +30280,7 @@
         <v>1256</v>
       </c>
       <c r="B1237" s="3" t="s">
-        <v>1256</v>
+        <v>415</v>
       </c>
       <c r="C1237" s="3">
         <v>99</v>
@@ -46791,14 +46918,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2750" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2750" t="s">
+    <row r="2750" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2750" s="3" t="s">
         <v>2794</v>
       </c>
-      <c r="B2750" t="s">
+      <c r="B2750" s="3" t="s">
         <v>2794</v>
       </c>
-      <c r="C2750">
+      <c r="C2750" s="3">
         <v>9</v>
       </c>
     </row>

</xml_diff>